<commit_message>
Fixed bug that caused Purity to not be calculated correctly
</commit_message>
<xml_diff>
--- a/Entwurf.xlsx
+++ b/Entwurf.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25831"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBE13471-ABB2-4716-9BCF-93BC2235D135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71EA5BB0-075C-48BF-9A3C-2FCA0DF03588}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vorbehandlungen" sheetId="1" r:id="rId1"/>
@@ -16450,7 +16450,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:M650"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A92" sqref="A92:A593"/>
     </sheetView>
   </sheetViews>
@@ -41298,8 +41298,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>

<commit_message>
Added products to Excel, minor other stuff
</commit_message>
<xml_diff>
--- a/Entwurf.xlsx
+++ b/Entwurf.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25928"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71EA5BB0-075C-48BF-9A3C-2FCA0DF03588}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{227C7E77-5BF1-4939-AB64-B5ED08432A15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" firstSheet="1" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" firstSheet="1" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Vorbehandlungen" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9308" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9380" uniqueCount="404">
   <si>
     <t>HDH Aufschluss</t>
   </si>
@@ -1752,8 +1752,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Tabelle2" displayName="Tabelle2" ref="A1:D351" totalsRowShown="0">
-  <autoFilter ref="A1:D351" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Tabelle2" displayName="Tabelle2" ref="A1:D387" totalsRowShown="0">
+  <autoFilter ref="A1:D387" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="Versuch"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="Produktfraktion"/>
@@ -1769,7 +1769,8 @@
   <autoFilter ref="A1:M650" xr:uid="{00000000-0009-0000-0100-000005000000}">
     <filterColumn colId="2">
       <filters>
-        <filter val="Trockene Zellen"/>
+        <filter val="Extrahierte Zellreste"/>
+        <filter val="PHA"/>
       </filters>
     </filterColumn>
     <filterColumn colId="5">
@@ -2786,7 +2787,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A114" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A160" sqref="A160"/>
+      <selection pane="bottomLeft" activeCell="F118" sqref="F118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -11727,10 +11728,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:D351"/>
+  <dimension ref="A1:D387"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A347" workbookViewId="0">
+      <selection activeCell="G350" sqref="G350"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -16438,6 +16439,294 @@
         <v>30.107099999999999</v>
       </c>
     </row>
+    <row r="352" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="A352" t="s">
+        <v>156</v>
+      </c>
+      <c r="B352" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="353" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A353" t="s">
+        <v>157</v>
+      </c>
+      <c r="B353" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="354" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A354" t="s">
+        <v>158</v>
+      </c>
+      <c r="B354" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="355" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A355" t="s">
+        <v>159</v>
+      </c>
+      <c r="B355" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="356" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A356" t="s">
+        <v>160</v>
+      </c>
+      <c r="B356" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="357" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A357" t="s">
+        <v>161</v>
+      </c>
+      <c r="B357" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="358" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A358" t="s">
+        <v>162</v>
+      </c>
+      <c r="B358" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="359" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A359" t="s">
+        <v>163</v>
+      </c>
+      <c r="B359" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="360" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A360" t="s">
+        <v>164</v>
+      </c>
+      <c r="B360" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="361" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A361" t="s">
+        <v>165</v>
+      </c>
+      <c r="B361" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="362" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A362" t="s">
+        <v>166</v>
+      </c>
+      <c r="B362" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="363" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A363" t="s">
+        <v>167</v>
+      </c>
+      <c r="B363" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="364" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A364" t="s">
+        <v>168</v>
+      </c>
+      <c r="B364" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="365" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A365" t="s">
+        <v>169</v>
+      </c>
+      <c r="B365" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="366" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A366" t="s">
+        <v>170</v>
+      </c>
+      <c r="B366" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="367" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A367" t="s">
+        <v>171</v>
+      </c>
+      <c r="B367" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="368" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A368" t="s">
+        <v>172</v>
+      </c>
+      <c r="B368" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="369" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A369" t="s">
+        <v>173</v>
+      </c>
+      <c r="B369" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="370" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A370" t="s">
+        <v>174</v>
+      </c>
+      <c r="B370" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="371" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A371" t="s">
+        <v>175</v>
+      </c>
+      <c r="B371" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="372" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A372" t="s">
+        <v>176</v>
+      </c>
+      <c r="B372" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="373" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A373" t="s">
+        <v>177</v>
+      </c>
+      <c r="B373" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="374" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A374" t="s">
+        <v>178</v>
+      </c>
+      <c r="B374" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="375" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A375" t="s">
+        <v>179</v>
+      </c>
+      <c r="B375" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="376" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A376" t="s">
+        <v>180</v>
+      </c>
+      <c r="B376" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="377" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A377" t="s">
+        <v>181</v>
+      </c>
+      <c r="B377" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="378" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A378" t="s">
+        <v>182</v>
+      </c>
+      <c r="B378" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="379" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A379" t="s">
+        <v>183</v>
+      </c>
+      <c r="B379" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="380" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A380" t="s">
+        <v>184</v>
+      </c>
+      <c r="B380" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="381" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A381" t="s">
+        <v>185</v>
+      </c>
+      <c r="B381" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="382" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A382" t="s">
+        <v>186</v>
+      </c>
+      <c r="B382" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="383" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A383" t="s">
+        <v>187</v>
+      </c>
+      <c r="B383" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="384" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A384" t="s">
+        <v>188</v>
+      </c>
+      <c r="B384" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="385" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A385" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="B385" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="386" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A386" t="s">
+        <v>190</v>
+      </c>
+      <c r="B386" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="387" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A387" t="s">
+        <v>191</v>
+      </c>
+      <c r="B387" t="s">
+        <v>82</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -16450,8 +16739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:M650"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A92" sqref="A92:A593"/>
+    <sheetView topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="I154" sqref="I154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -16512,7 +16801,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="2" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A2">
         <v>1</v>
       </c>
@@ -16550,7 +16839,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="3" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>2</v>
       </c>
@@ -16588,7 +16877,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="4" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>3</v>
       </c>
@@ -16626,7 +16915,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="5" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>4</v>
       </c>
@@ -16664,7 +16953,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="6" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>5</v>
       </c>
@@ -16702,7 +16991,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="7" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>6</v>
       </c>
@@ -16740,7 +17029,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="8" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>7</v>
       </c>
@@ -16778,7 +17067,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="9" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>8</v>
       </c>
@@ -16816,7 +17105,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="10" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>9</v>
       </c>
@@ -16854,7 +17143,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="11" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>10</v>
       </c>
@@ -16892,7 +17181,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="12" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>11</v>
       </c>
@@ -16930,7 +17219,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="13" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>12</v>
       </c>
@@ -17880,7 +18169,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="38" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A38">
         <v>37</v>
       </c>
@@ -17918,7 +18207,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="39" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A39">
         <v>38</v>
       </c>
@@ -17956,7 +18245,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="40" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A40">
         <v>39</v>
       </c>
@@ -17994,7 +18283,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="41" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A41">
         <v>40</v>
       </c>
@@ -18032,7 +18321,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="42" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A42">
         <v>41</v>
       </c>
@@ -18070,7 +18359,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="43" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A43">
         <v>42</v>
       </c>
@@ -18108,7 +18397,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="44" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A44">
         <v>43</v>
       </c>
@@ -18146,7 +18435,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="45" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A45">
         <v>44</v>
       </c>
@@ -18184,7 +18473,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="46" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A46">
         <v>45</v>
       </c>
@@ -18222,7 +18511,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="47" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A47">
         <v>46</v>
       </c>
@@ -18336,7 +18625,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="50" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A50">
         <v>49</v>
       </c>
@@ -18374,7 +18663,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="51" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A51">
         <v>50</v>
       </c>
@@ -18792,7 +19081,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="62" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A62">
         <v>61</v>
       </c>
@@ -18874,7 +19163,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="64" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A64">
         <v>63</v>
       </c>
@@ -18956,7 +19245,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="66" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A66">
         <v>65</v>
       </c>
@@ -19038,7 +19327,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="68" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A68">
         <v>67</v>
       </c>
@@ -19114,7 +19403,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="70" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A70">
         <v>69</v>
       </c>
@@ -19190,7 +19479,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="72" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A72">
         <v>71</v>
       </c>
@@ -19257,7 +19546,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="74" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A74">
         <v>73</v>
       </c>
@@ -19324,7 +19613,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="76" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A76">
         <v>75</v>
       </c>
@@ -19403,7 +19692,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="78" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A78">
         <v>77</v>
       </c>
@@ -19479,7 +19768,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="80" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A80">
         <v>79</v>
       </c>
@@ -19558,7 +19847,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="82" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A82">
         <v>81</v>
       </c>
@@ -19634,7 +19923,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="84" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A84">
         <v>83</v>
       </c>
@@ -19672,7 +19961,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="85" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A85">
         <v>84</v>
       </c>
@@ -19710,7 +19999,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="86" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A86">
         <v>85</v>
       </c>
@@ -19748,7 +20037,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="87" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A87">
         <v>86</v>
       </c>
@@ -19920,7 +20209,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
       <c r="A92">
         <v>91</v>
       </c>
@@ -19961,7 +20250,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
       <c r="A93">
         <v>92</v>
       </c>
@@ -20084,7 +20373,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
       <c r="A96">
         <v>95</v>
       </c>
@@ -20122,7 +20411,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
       <c r="A97">
         <v>96</v>
       </c>
@@ -20236,7 +20525,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
       <c r="A100">
         <v>99</v>
       </c>
@@ -20274,7 +20563,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
       <c r="A101">
         <v>100</v>
       </c>
@@ -20391,7 +20680,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
       <c r="A104">
         <v>103</v>
       </c>
@@ -20473,7 +20762,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
       <c r="A106">
         <v>105</v>
       </c>
@@ -20552,7 +20841,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
       <c r="A108">
         <v>107</v>
       </c>
@@ -20628,7 +20917,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="110" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A110">
         <v>109</v>
       </c>
@@ -20666,7 +20955,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="111" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A111">
         <v>110</v>
       </c>
@@ -21190,7 +21479,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="124" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A124">
         <v>123</v>
       </c>
@@ -21228,7 +21517,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="125" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A125">
         <v>124</v>
       </c>
@@ -21342,7 +21631,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="128" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A128">
         <v>127</v>
       </c>
@@ -21380,7 +21669,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="129" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A129">
         <v>128</v>
       </c>
@@ -21476,7 +21765,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="132" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A132">
         <v>131</v>
       </c>
@@ -21517,7 +21806,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="133" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A133">
         <v>132</v>
       </c>
@@ -21593,7 +21882,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="135" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A135">
         <v>134</v>
       </c>
@@ -21634,7 +21923,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="136" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A136">
         <v>135</v>
       </c>
@@ -21710,7 +21999,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="138" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A138">
         <v>137</v>
       </c>
@@ -21751,7 +22040,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="139" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A139">
         <v>138</v>
       </c>
@@ -21827,7 +22116,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="141" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A141">
         <v>140</v>
       </c>
@@ -21868,7 +22157,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="142" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A142">
         <v>141</v>
       </c>
@@ -21944,7 +22233,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="144" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A144">
         <v>143</v>
       </c>
@@ -21985,7 +22274,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="145" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A145">
         <v>144</v>
       </c>
@@ -22061,7 +22350,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="147" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A147">
         <v>146</v>
       </c>
@@ -22102,7 +22391,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="148" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A148">
         <v>147</v>
       </c>
@@ -22178,7 +22467,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="150" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A150">
         <v>149</v>
       </c>
@@ -22219,7 +22508,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="151" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A151">
         <v>150</v>
       </c>
@@ -22295,7 +22584,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="153" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A153">
         <v>152</v>
       </c>
@@ -22336,7 +22625,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="154" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A154">
         <v>153</v>
       </c>
@@ -22412,7 +22701,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="156" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A156">
         <v>155</v>
       </c>
@@ -22453,7 +22742,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="157" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A157">
         <v>156</v>
       </c>
@@ -22494,7 +22783,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="158" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A158">
         <v>157</v>
       </c>
@@ -22535,7 +22824,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="159" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A159">
         <v>158</v>
       </c>
@@ -22611,7 +22900,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="161" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
       <c r="A161">
         <v>160</v>
       </c>
@@ -22652,7 +22941,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="162" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
       <c r="A162">
         <v>161</v>
       </c>
@@ -22728,7 +23017,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="164" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A164">
         <v>163</v>
       </c>
@@ -22766,7 +23055,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="165" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A165">
         <v>164</v>
       </c>
@@ -22862,7 +23151,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="168" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A168">
         <v>167</v>
       </c>
@@ -22900,7 +23189,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="169" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A169">
         <v>168</v>
       </c>
@@ -22996,7 +23285,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="172" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A172">
         <v>171</v>
       </c>
@@ -23034,7 +23323,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="173" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A173">
         <v>172</v>
       </c>
@@ -23130,7 +23419,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="176" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A176">
         <v>175</v>
       </c>
@@ -23168,7 +23457,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="177" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="177" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A177">
         <v>176</v>
       </c>
@@ -23264,7 +23553,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="180" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="180" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
       <c r="A180">
         <v>179</v>
       </c>
@@ -23305,7 +23594,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="181" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="181" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
       <c r="A181">
         <v>180</v>
       </c>
@@ -23346,7 +23635,7 @@
         <v>255</v>
       </c>
     </row>
-    <row r="182" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="182" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A182">
         <v>181</v>
       </c>
@@ -23384,7 +23673,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="183" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="183" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A183">
         <v>182</v>
       </c>
@@ -23480,7 +23769,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="186" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="186" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A186">
         <v>185</v>
       </c>
@@ -23518,7 +23807,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="187" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="187" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A187">
         <v>186</v>
       </c>
@@ -23614,7 +23903,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="190" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="190" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A190">
         <v>189</v>
       </c>
@@ -23643,7 +23932,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="191" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="191" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A191">
         <v>190</v>
       </c>
@@ -23730,7 +24019,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="194" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="194" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A194">
         <v>193</v>
       </c>
@@ -23768,7 +24057,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="195" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="195" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A195">
         <v>194</v>
       </c>
@@ -23864,7 +24153,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="198" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="198" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A198">
         <v>197</v>
       </c>
@@ -23893,7 +24182,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="199" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="199" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A199">
         <v>198</v>
       </c>
@@ -23980,7 +24269,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="202" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="202" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A202">
         <v>201</v>
       </c>
@@ -24018,7 +24307,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="203" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="203" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A203">
         <v>202</v>
       </c>
@@ -24114,7 +24403,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="206" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="206" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A206">
         <v>205</v>
       </c>
@@ -24143,7 +24432,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="207" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="207" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A207">
         <v>206</v>
       </c>
@@ -24230,7 +24519,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="210" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="210" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A210">
         <v>209</v>
       </c>
@@ -24268,7 +24557,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="211" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="211" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A211">
         <v>210</v>
       </c>
@@ -24364,7 +24653,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="214" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="214" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A214">
         <v>213</v>
       </c>
@@ -24393,7 +24682,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="215" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="215" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A215">
         <v>214</v>
       </c>
@@ -24480,7 +24769,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="218" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="218" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A218">
         <v>217</v>
       </c>
@@ -24518,7 +24807,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="219" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="219" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A219">
         <v>218</v>
       </c>
@@ -24614,7 +24903,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="222" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="222" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A222">
         <v>221</v>
       </c>
@@ -24652,7 +24941,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="223" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="223" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A223">
         <v>222</v>
       </c>
@@ -24795,7 +25084,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="227" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="227" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A227">
         <v>226</v>
       </c>
@@ -24836,7 +25125,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="228" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="228" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A228">
         <v>227</v>
       </c>
@@ -24877,7 +25166,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="229" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="229" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A229">
         <v>228</v>
       </c>
@@ -24918,7 +25207,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="230" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="230" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A230">
         <v>229</v>
       </c>
@@ -24959,7 +25248,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="231" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="231" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A231">
         <v>230</v>
       </c>
@@ -24997,7 +25286,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="232" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="232" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A232">
         <v>231</v>
       </c>
@@ -25035,7 +25324,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="233" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="233" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A233">
         <v>236</v>
       </c>
@@ -25076,7 +25365,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="234" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="234" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A234">
         <v>237</v>
       </c>
@@ -25117,7 +25406,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="235" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="235" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A235">
         <v>238</v>
       </c>
@@ -25158,7 +25447,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="236" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="236" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A236">
         <v>239</v>
       </c>
@@ -25199,7 +25488,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="237" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="237" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A237">
         <v>240</v>
       </c>
@@ -25240,7 +25529,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="238" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="238" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A238">
         <v>241</v>
       </c>
@@ -25281,7 +25570,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="239" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="239" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A239">
         <v>242</v>
       </c>
@@ -25322,7 +25611,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="240" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="240" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A240">
         <v>243</v>
       </c>
@@ -25363,7 +25652,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="241" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="241" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A241">
         <v>244</v>
       </c>
@@ -25404,7 +25693,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="242" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="242" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A242">
         <v>245</v>
       </c>
@@ -25445,7 +25734,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="243" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="243" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A243">
         <v>246</v>
       </c>
@@ -25486,7 +25775,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="244" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="244" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A244">
         <v>247</v>
       </c>
@@ -25527,7 +25816,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="245" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="245" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A245">
         <v>248</v>
       </c>
@@ -25568,7 +25857,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="246" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="246" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A246">
         <v>249</v>
       </c>
@@ -25609,7 +25898,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="247" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="247" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A247">
         <v>250</v>
       </c>
@@ -25650,7 +25939,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="248" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="248" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A248">
         <v>251</v>
       </c>
@@ -25691,7 +25980,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="249" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="249" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A249">
         <v>252</v>
       </c>
@@ -25732,7 +26021,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="250" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="250" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A250">
         <v>253</v>
       </c>
@@ -25773,7 +26062,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="251" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="251" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A251">
         <v>254</v>
       </c>
@@ -25814,7 +26103,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="252" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="252" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A252">
         <v>255</v>
       </c>
@@ -25855,7 +26144,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="253" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="253" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A253">
         <v>256</v>
       </c>
@@ -25896,7 +26185,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="254" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="254" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A254">
         <v>257</v>
       </c>
@@ -25937,7 +26226,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="255" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="255" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A255">
         <v>258</v>
       </c>
@@ -25978,7 +26267,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="256" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="256" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A256">
         <v>259</v>
       </c>
@@ -26019,7 +26308,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="257" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="257" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A257">
         <v>260</v>
       </c>
@@ -26060,7 +26349,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="258" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="258" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A258">
         <v>261</v>
       </c>
@@ -26101,7 +26390,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="259" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="259" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A259">
         <v>262</v>
       </c>
@@ -26142,7 +26431,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="260" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="260" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A260">
         <v>263</v>
       </c>
@@ -26798,7 +27087,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="276" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="276" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
       <c r="A276">
         <v>279</v>
       </c>
@@ -26839,7 +27128,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="277" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="277" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
       <c r="A277">
         <v>280</v>
       </c>
@@ -26880,7 +27169,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="278" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="278" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
       <c r="A278">
         <v>281</v>
       </c>
@@ -26921,7 +27210,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="279" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="279" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A279">
         <v>282</v>
       </c>
@@ -26962,7 +27251,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="280" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="280" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A280">
         <v>283</v>
       </c>
@@ -27003,7 +27292,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="281" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="281" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A281">
         <v>284</v>
       </c>
@@ -27044,7 +27333,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="282" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="282" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A282">
         <v>285</v>
       </c>
@@ -27085,7 +27374,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="283" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="283" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A283">
         <v>286</v>
       </c>
@@ -27126,7 +27415,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="284" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="284" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A284">
         <v>287</v>
       </c>
@@ -27167,7 +27456,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="285" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="285" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A285">
         <v>288</v>
       </c>
@@ -27208,7 +27497,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="286" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="286" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A286">
         <v>289</v>
       </c>
@@ -27249,7 +27538,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="287" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="287" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A287">
         <v>290</v>
       </c>
@@ -27290,7 +27579,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="288" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="288" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A288">
         <v>291</v>
       </c>
@@ -27331,7 +27620,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="289" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="289" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A289">
         <v>292</v>
       </c>
@@ -27372,7 +27661,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="290" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="290" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A290">
         <v>293</v>
       </c>
@@ -27413,7 +27702,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="291" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="291" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A291">
         <v>294</v>
       </c>
@@ -27700,7 +27989,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="298" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="298" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A298">
         <v>301</v>
       </c>
@@ -27741,7 +28030,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="299" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="299" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A299">
         <v>302</v>
       </c>
@@ -27782,7 +28071,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="300" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="300" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A300">
         <v>303</v>
       </c>
@@ -27823,7 +28112,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="301" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="301" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A301">
         <v>304</v>
       </c>
@@ -27864,7 +28153,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="302" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="302" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A302">
         <v>305</v>
       </c>
@@ -27905,7 +28194,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="303" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="303" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A303">
         <v>306</v>
       </c>
@@ -27946,7 +28235,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="304" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="304" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A304">
         <v>307</v>
       </c>
@@ -27987,7 +28276,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="305" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="305" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A305">
         <v>308</v>
       </c>
@@ -28028,7 +28317,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="306" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="306" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A306">
         <v>309</v>
       </c>
@@ -28069,7 +28358,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="307" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="307" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A307">
         <v>310</v>
       </c>
@@ -28110,7 +28399,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="308" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="308" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A308">
         <v>311</v>
       </c>
@@ -28151,7 +28440,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="309" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="309" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A309">
         <v>312</v>
       </c>
@@ -28192,7 +28481,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="310" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="310" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A310">
         <v>313</v>
       </c>
@@ -28233,7 +28522,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="311" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="311" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A311">
         <v>314</v>
       </c>
@@ -28274,7 +28563,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="312" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="312" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A312">
         <v>315</v>
       </c>
@@ -28315,7 +28604,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="313" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="313" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A313">
         <v>316</v>
       </c>
@@ -28356,7 +28645,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="314" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="314" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A314">
         <v>317</v>
       </c>
@@ -28397,7 +28686,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="315" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="315" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A315">
         <v>318</v>
       </c>
@@ -28438,7 +28727,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="316" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="316" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A316">
         <v>319</v>
       </c>
@@ -28479,7 +28768,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="317" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="317" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A317">
         <v>320</v>
       </c>
@@ -28520,7 +28809,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="318" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="318" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A318">
         <v>321</v>
       </c>
@@ -28561,7 +28850,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="319" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="319" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A319">
         <v>322</v>
       </c>
@@ -28602,7 +28891,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="320" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="320" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A320">
         <v>323</v>
       </c>
@@ -28643,7 +28932,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="321" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="321" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A321">
         <v>324</v>
       </c>
@@ -28684,7 +28973,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="322" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="322" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A322">
         <v>325</v>
       </c>
@@ -28725,7 +29014,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="323" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="323" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A323">
         <v>326</v>
       </c>
@@ -28766,7 +29055,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="324" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="324" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A324">
         <v>327</v>
       </c>
@@ -28807,7 +29096,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="325" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="325" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A325">
         <v>328</v>
       </c>
@@ -28848,7 +29137,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="326" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="326" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A326">
         <v>329</v>
       </c>
@@ -28889,7 +29178,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="327" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="327" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A327">
         <v>330</v>
       </c>
@@ -28930,7 +29219,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="328" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="328" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A328">
         <v>331</v>
       </c>
@@ -28971,7 +29260,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="329" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="329" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A329">
         <v>332</v>
       </c>
@@ -29012,7 +29301,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="330" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="330" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A330">
         <v>333</v>
       </c>
@@ -29299,7 +29588,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="337" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="337" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
       <c r="A337">
         <v>340</v>
       </c>
@@ -29340,7 +29629,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="338" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="338" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A338">
         <v>341</v>
       </c>
@@ -29381,7 +29670,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="339" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="339" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A339">
         <v>342</v>
       </c>
@@ -29422,7 +29711,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="340" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="340" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A340">
         <v>343</v>
       </c>
@@ -29463,7 +29752,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="341" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="341" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A341">
         <v>344</v>
       </c>
@@ -29504,7 +29793,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="342" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="342" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A342">
         <v>345</v>
       </c>
@@ -29545,7 +29834,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="343" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="343" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A343">
         <v>346</v>
       </c>
@@ -29586,7 +29875,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="344" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="344" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A344">
         <v>347</v>
       </c>
@@ -29627,7 +29916,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="345" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="345" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A345">
         <v>348</v>
       </c>
@@ -29668,7 +29957,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="346" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="346" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A346">
         <v>349</v>
       </c>
@@ -29709,7 +29998,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="347" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="347" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A347">
         <v>350</v>
       </c>
@@ -29750,7 +30039,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="348" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="348" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A348">
         <v>351</v>
       </c>
@@ -29791,7 +30080,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="349" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="349" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A349">
         <v>352</v>
       </c>
@@ -29832,7 +30121,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="350" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="350" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A350">
         <v>353</v>
       </c>
@@ -29873,7 +30162,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="351" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="351" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A351">
         <v>354</v>
       </c>
@@ -29914,7 +30203,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="352" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="352" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A352">
         <v>355</v>
       </c>
@@ -29955,7 +30244,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="353" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="353" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A353">
         <v>356</v>
       </c>
@@ -29996,7 +30285,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="354" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="354" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A354">
         <v>357</v>
       </c>
@@ -30037,7 +30326,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="355" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="355" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A355">
         <v>358</v>
       </c>
@@ -30078,7 +30367,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="356" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="356" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A356">
         <v>359</v>
       </c>
@@ -30119,7 +30408,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="357" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="357" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A357">
         <v>360</v>
       </c>
@@ -30160,7 +30449,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="358" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="358" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A358">
         <v>361</v>
       </c>
@@ -30201,7 +30490,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="359" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="359" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A359">
         <v>362</v>
       </c>
@@ -30242,7 +30531,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="360" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="360" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A360">
         <v>363</v>
       </c>
@@ -30283,7 +30572,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="361" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="361" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A361">
         <v>364</v>
       </c>
@@ -30324,7 +30613,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="362" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="362" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A362">
         <v>365</v>
       </c>
@@ -30365,7 +30654,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="363" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="363" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A363">
         <v>366</v>
       </c>
@@ -30406,7 +30695,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="364" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="364" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A364">
         <v>367</v>
       </c>
@@ -30447,7 +30736,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="365" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="365" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A365">
         <v>368</v>
       </c>
@@ -30488,7 +30777,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="366" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="366" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A366">
         <v>369</v>
       </c>
@@ -30529,7 +30818,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="367" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="367" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A367">
         <v>370</v>
       </c>
@@ -30570,7 +30859,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="368" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="368" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A368">
         <v>371</v>
       </c>
@@ -30611,7 +30900,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="369" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="369" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A369">
         <v>372</v>
       </c>
@@ -30652,7 +30941,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="370" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="370" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A370">
         <v>373</v>
       </c>
@@ -30693,7 +30982,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="371" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="371" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A371">
         <v>374</v>
       </c>
@@ -30734,7 +31023,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="372" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="372" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A372">
         <v>375</v>
       </c>
@@ -30775,7 +31064,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="373" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="373" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A373">
         <v>376</v>
       </c>
@@ -30816,7 +31105,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="374" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="374" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A374">
         <v>377</v>
       </c>
@@ -30857,7 +31146,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="375" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="375" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A375">
         <v>378</v>
       </c>
@@ -30898,7 +31187,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="376" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="376" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A376">
         <v>379</v>
       </c>
@@ -30939,7 +31228,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="377" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="377" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A377">
         <v>380</v>
       </c>
@@ -30980,7 +31269,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="378" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="378" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A378">
         <v>381</v>
       </c>
@@ -31021,7 +31310,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="379" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="379" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A379">
         <v>382</v>
       </c>
@@ -31062,7 +31351,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="380" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="380" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A380">
         <v>383</v>
       </c>
@@ -31103,7 +31392,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="381" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="381" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A381">
         <v>384</v>
       </c>
@@ -31144,7 +31433,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="382" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="382" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A382">
         <v>385</v>
       </c>
@@ -31185,7 +31474,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="383" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="383" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A383">
         <v>386</v>
       </c>
@@ -31226,7 +31515,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="384" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="384" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A384">
         <v>387</v>
       </c>
@@ -31267,7 +31556,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="385" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="385" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A385">
         <v>388</v>
       </c>
@@ -31308,7 +31597,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="386" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="386" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A386">
         <v>389</v>
       </c>
@@ -32374,7 +32663,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="412" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="412" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A412">
         <v>415</v>
       </c>
@@ -32415,7 +32704,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="413" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="413" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A413">
         <v>416</v>
       </c>
@@ -32456,7 +32745,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="414" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="414" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A414">
         <v>417</v>
       </c>
@@ -32497,7 +32786,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="415" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="415" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A415">
         <v>418</v>
       </c>
@@ -32538,7 +32827,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="416" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="416" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A416">
         <v>419</v>
       </c>
@@ -32579,7 +32868,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="417" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="417" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A417">
         <v>420</v>
       </c>
@@ -32620,7 +32909,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="418" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="418" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A418">
         <v>421</v>
       </c>
@@ -32661,7 +32950,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="419" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="419" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A419">
         <v>422</v>
       </c>
@@ -32702,7 +32991,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="420" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="420" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A420">
         <v>423</v>
       </c>
@@ -32743,7 +33032,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="421" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="421" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A421">
         <v>424</v>
       </c>
@@ -32784,7 +33073,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="422" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="422" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A422">
         <v>425</v>
       </c>
@@ -32825,7 +33114,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="423" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="423" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A423">
         <v>426</v>
       </c>
@@ -32866,7 +33155,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="424" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="424" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A424">
         <v>427</v>
       </c>
@@ -32907,7 +33196,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="425" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="425" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A425">
         <v>428</v>
       </c>
@@ -32948,7 +33237,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="426" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="426" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A426">
         <v>429</v>
       </c>
@@ -32989,7 +33278,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="427" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="427" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A427">
         <v>430</v>
       </c>
@@ -33030,7 +33319,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="428" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="428" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A428">
         <v>431</v>
       </c>
@@ -33071,7 +33360,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="429" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="429" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A429">
         <v>432</v>
       </c>
@@ -33112,7 +33401,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="430" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="430" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A430">
         <v>433</v>
       </c>
@@ -33153,7 +33442,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="431" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="431" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A431">
         <v>434</v>
       </c>
@@ -33194,7 +33483,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="432" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="432" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A432">
         <v>435</v>
       </c>
@@ -33235,7 +33524,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="433" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="433" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A433">
         <v>436</v>
       </c>
@@ -33276,7 +33565,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="434" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="434" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A434">
         <v>437</v>
       </c>
@@ -33317,7 +33606,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="435" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="435" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A435">
         <v>438</v>
       </c>
@@ -33358,7 +33647,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="436" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="436" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A436">
         <v>439</v>
       </c>
@@ -33399,7 +33688,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="437" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="437" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A437">
         <v>440</v>
       </c>
@@ -33440,7 +33729,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="438" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="438" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A438">
         <v>441</v>
       </c>
@@ -33481,7 +33770,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="439" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="439" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A439">
         <v>442</v>
       </c>
@@ -33522,7 +33811,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="440" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="440" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A440">
         <v>443</v>
       </c>
@@ -33563,7 +33852,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="441" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="441" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A441">
         <v>444</v>
       </c>
@@ -33604,7 +33893,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="442" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="442" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A442">
         <v>445</v>
       </c>
@@ -33645,7 +33934,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="443" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="443" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A443">
         <v>446</v>
       </c>
@@ -33686,7 +33975,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="444" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="444" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A444">
         <v>447</v>
       </c>
@@ -33727,7 +34016,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="445" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="445" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A445">
         <v>448</v>
       </c>
@@ -33768,7 +34057,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="446" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="446" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A446">
         <v>449</v>
       </c>
@@ -33809,7 +34098,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="447" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="447" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A447">
         <v>450</v>
       </c>
@@ -33850,7 +34139,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="448" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="448" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A448">
         <v>451</v>
       </c>
@@ -33891,7 +34180,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="449" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="449" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A449">
         <v>452</v>
       </c>
@@ -33932,7 +34221,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="450" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="450" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A450">
         <v>453</v>
       </c>
@@ -33973,7 +34262,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="451" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="451" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A451">
         <v>454</v>
       </c>
@@ -37409,7 +37698,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="549" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="549" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A549">
         <v>552</v>
       </c>
@@ -37447,7 +37736,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="550" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="550" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A550">
         <v>553</v>
       </c>
@@ -37485,7 +37774,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="551" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="551" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A551">
         <v>554</v>
       </c>
@@ -37523,7 +37812,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="552" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="552" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A552">
         <v>555</v>
       </c>
@@ -37561,7 +37850,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="553" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="553" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A553">
         <v>556</v>
       </c>
@@ -37599,7 +37888,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="554" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="554" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A554">
         <v>557</v>
       </c>
@@ -37637,7 +37926,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="555" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="555" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A555">
         <v>558</v>
       </c>
@@ -37675,7 +37964,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="556" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="556" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A556">
         <v>559</v>
       </c>
@@ -37713,7 +38002,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="557" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="557" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A557">
         <v>560</v>
       </c>
@@ -37751,7 +38040,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="558" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="558" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A558">
         <v>561</v>
       </c>
@@ -37789,7 +38078,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="559" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="559" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A559">
         <v>562</v>
       </c>
@@ -37827,7 +38116,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="560" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="560" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A560">
         <v>563</v>
       </c>
@@ -37865,7 +38154,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="561" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="561" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A561">
         <v>564</v>
       </c>
@@ -37903,7 +38192,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="562" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="562" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A562">
         <v>565</v>
       </c>
@@ -37941,7 +38230,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="563" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="563" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A563">
         <v>566</v>
       </c>
@@ -37979,7 +38268,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="564" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="564" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A564">
         <v>567</v>
       </c>
@@ -38017,7 +38306,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="565" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="565" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A565">
         <v>568</v>
       </c>
@@ -38055,7 +38344,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="566" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="566" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A566">
         <v>569</v>
       </c>
@@ -38093,7 +38382,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="567" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="567" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A567">
         <v>570</v>
       </c>
@@ -38131,7 +38420,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="568" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="568" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A568">
         <v>571</v>
       </c>
@@ -38169,7 +38458,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="569" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="569" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A569">
         <v>572</v>
       </c>
@@ -38207,7 +38496,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="570" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="570" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A570">
         <v>573</v>
       </c>
@@ -38245,7 +38534,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="571" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="571" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A571">
         <v>574</v>
       </c>
@@ -38283,7 +38572,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="572" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="572" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A572">
         <v>575</v>
       </c>
@@ -38321,7 +38610,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="573" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="573" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A573">
         <v>576</v>
       </c>
@@ -38359,7 +38648,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="574" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="574" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A574">
         <v>577</v>
       </c>
@@ -38397,7 +38686,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="575" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="575" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A575">
         <v>578</v>
       </c>
@@ -38435,7 +38724,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="576" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="576" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A576">
         <v>579</v>
       </c>
@@ -38473,7 +38762,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="577" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="577" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A577">
         <v>580</v>
       </c>
@@ -38511,7 +38800,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="578" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="578" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A578">
         <v>581</v>
       </c>
@@ -38549,7 +38838,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="579" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="579" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A579">
         <v>582</v>
       </c>
@@ -38587,7 +38876,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="580" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="580" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A580">
         <v>583</v>
       </c>
@@ -38625,7 +38914,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="581" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="581" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A581">
         <v>584</v>
       </c>
@@ -38663,7 +38952,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="582" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="582" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A582">
         <v>585</v>
       </c>
@@ -38701,7 +38990,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="583" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="583" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A583">
         <v>586</v>
       </c>
@@ -38739,7 +39028,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="584" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="584" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A584">
         <v>587</v>
       </c>
@@ -38777,7 +39066,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="585" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="585" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A585">
         <v>588</v>
       </c>
@@ -38815,7 +39104,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="586" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="586" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A586">
         <v>589</v>
       </c>
@@ -38853,7 +39142,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="587" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="587" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A587">
         <v>590</v>
       </c>
@@ -38891,7 +39180,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="588" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="588" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A588">
         <v>591</v>
       </c>
@@ -38929,7 +39218,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="589" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="589" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A589">
         <v>592</v>
       </c>
@@ -38967,7 +39256,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="590" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="590" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A590">
         <v>593</v>
       </c>
@@ -39005,7 +39294,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="591" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="591" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A591">
         <v>594</v>
       </c>
@@ -39043,7 +39332,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="592" spans="1:12" hidden="1" x14ac:dyDescent="0.45">
+    <row r="592" spans="1:12" x14ac:dyDescent="0.45">
       <c r="A592">
         <v>595</v>
       </c>
@@ -39081,7 +39370,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="593" spans="1:13" x14ac:dyDescent="0.45">
+    <row r="593" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
       <c r="A593">
         <v>596</v>
       </c>
@@ -39347,7 +39636,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="600" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="600" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A600">
         <v>603</v>
       </c>
@@ -39385,7 +39674,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="601" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="601" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A601">
         <v>604</v>
       </c>
@@ -40183,7 +40472,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="622" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="622" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A622">
         <v>625</v>
       </c>
@@ -40221,7 +40510,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="623" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="623" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A623">
         <v>626</v>
       </c>
@@ -40259,7 +40548,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="624" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="624" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A624">
         <v>627</v>
       </c>
@@ -40297,7 +40586,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="625" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="625" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A625">
         <v>628</v>
       </c>
@@ -40335,7 +40624,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="626" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="626" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A626">
         <v>629</v>
       </c>
@@ -40373,7 +40662,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="627" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="627" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A627">
         <v>630</v>
       </c>
@@ -40411,7 +40700,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="628" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="628" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A628">
         <v>631</v>
       </c>
@@ -40449,7 +40738,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="629" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="629" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A629">
         <v>632</v>
       </c>
@@ -40487,7 +40776,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="630" spans="1:13" hidden="1" x14ac:dyDescent="0.45">
+    <row r="630" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A630">
         <v>633</v>
       </c>
@@ -41298,7 +41587,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J17" sqref="J17"/>
     </sheetView>
   </sheetViews>

</xml_diff>